<commit_message>
Created the Data provider utility for excel data that is used in Create Job API test
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/PhoenixTestData.xlsx
+++ b/src/test/resources/testData/PhoenixTestData.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tulinag/eclipse-workspace/PhoenixTestAutomationFramework/src/test/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E54AFFD-CABD-114C-A74D-8F63D444C27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A3346F-BD3A-A94D-A786-3B13C2232BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{B7643BA3-8AA4-E84C-AEE3-A7B3D9579004}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33500" windowHeight="21100" activeTab="1" xr2:uid="{B7643BA3-8AA4-E84C-AEE3-A7B3D9579004}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateJobTestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>username</t>
   </si>
@@ -35,13 +36,148 @@
   </si>
   <si>
     <t>iamsup</t>
+  </si>
+  <si>
+    <t>mst_service_location_id</t>
+  </si>
+  <si>
+    <t>mst_platform_id</t>
+  </si>
+  <si>
+    <t>mst_warrenty_status_id</t>
+  </si>
+  <si>
+    <t>mst_oem_id</t>
+  </si>
+  <si>
+    <t>customer__first_name</t>
+  </si>
+  <si>
+    <t>customer__last_name</t>
+  </si>
+  <si>
+    <t>customer__mobile_number</t>
+  </si>
+  <si>
+    <t>customer__mobile_number_alt</t>
+  </si>
+  <si>
+    <t>customer__email_id</t>
+  </si>
+  <si>
+    <t>customer__email_id_alt</t>
+  </si>
+  <si>
+    <t>customer_address__flat_number</t>
+  </si>
+  <si>
+    <t>customer_address__apartment_name</t>
+  </si>
+  <si>
+    <t>customer_address__street_name</t>
+  </si>
+  <si>
+    <t>customer_address__landmark</t>
+  </si>
+  <si>
+    <t>customer_address__area</t>
+  </si>
+  <si>
+    <t>customer_address__pincode</t>
+  </si>
+  <si>
+    <t>customer_address__country</t>
+  </si>
+  <si>
+    <t>customer_address__state</t>
+  </si>
+  <si>
+    <t>customer_product__dop</t>
+  </si>
+  <si>
+    <t>customer_product__serial_number</t>
+  </si>
+  <si>
+    <t>customer_product__imei1</t>
+  </si>
+  <si>
+    <t>customer_product__imei2</t>
+  </si>
+  <si>
+    <t>customer_product__popurl</t>
+  </si>
+  <si>
+    <t>customer_product__product_id</t>
+  </si>
+  <si>
+    <t>customer_product__mst_model_id</t>
+  </si>
+  <si>
+    <t>problems__id</t>
+  </si>
+  <si>
+    <t>problems__remark</t>
+  </si>
+  <si>
+    <t>Maiya</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>464-509-3987</t>
+  </si>
+  <si>
+    <t>Ismael.Bauch@hotmail.com</t>
+  </si>
+  <si>
+    <t>c 304</t>
+  </si>
+  <si>
+    <t>Jupiter</t>
+  </si>
+  <si>
+    <t>MG road</t>
+  </si>
+  <si>
+    <t>Bangur Nagar</t>
+  </si>
+  <si>
+    <t>Goregaon West</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>2025-04-06T18:30:00.000Z</t>
+  </si>
+  <si>
+    <t>Battery Issue</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Schmidt</t>
+  </si>
+  <si>
+    <t>39556938683600</t>
+  </si>
+  <si>
+    <t>29526938683600</t>
+  </si>
+  <si>
+    <t>464-509-3989</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +311,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -518,8 +660,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -897,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302BF737-74A1-AE48-BE31-B49FC56EB46C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -938,4 +1082,331 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB68402-FCE6-B44D-B21D-BB2F55D5AA88}">
+  <dimension ref="A1:AN3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:W3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="16" width="22.1640625" customWidth="1"/>
+    <col min="17" max="17" width="27" customWidth="1"/>
+    <col min="18" max="18" width="40.33203125" customWidth="1"/>
+    <col min="19" max="19" width="23.33203125" customWidth="1"/>
+    <col min="20" max="20" width="29" customWidth="1"/>
+    <col min="21" max="21" width="38.33203125" customWidth="1"/>
+    <col min="22" max="22" width="31.5" customWidth="1"/>
+    <col min="23" max="23" width="21" customWidth="1"/>
+    <col min="24" max="24" width="22.6640625" customWidth="1"/>
+    <col min="25" max="25" width="42.5" customWidth="1"/>
+    <col min="26" max="26" width="18.83203125" customWidth="1"/>
+    <col min="27" max="27" width="17" customWidth="1"/>
+    <col min="28" max="28" width="15.1640625" customWidth="1"/>
+    <col min="29" max="29" width="29.6640625" customWidth="1"/>
+    <col min="30" max="30" width="26.6640625" customWidth="1"/>
+    <col min="31" max="31" width="26.1640625" customWidth="1"/>
+    <col min="32" max="32" width="31.33203125" customWidth="1"/>
+    <col min="33" max="33" width="38.5" customWidth="1"/>
+    <col min="34" max="34" width="29" customWidth="1"/>
+    <col min="35" max="35" width="45.1640625" customWidth="1"/>
+    <col min="36" max="36" width="48.1640625" customWidth="1"/>
+    <col min="40" max="40" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2">
+        <v>411039</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AL2">
+        <v>1</v>
+      </c>
+      <c r="AM2">
+        <v>1</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC3">
+        <v>411039</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>1</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>